<commit_message>
Update Patient Example d560f279404f0f4d31a528608029274d6e6355c8
</commit_message>
<xml_diff>
--- a/303-exemple---création-dun-exemple-de-cas-dusage-ssiad/ig/StructureDefinition-tddui-birth-order.xlsx
+++ b/303-exemple---création-dun-exemple-de-cas-dusage-ssiad/ig/StructureDefinition-tddui-birth-order.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-28T14:45:11+00:00</t>
+    <t>2025-07-29T07:14:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -129,7 +129,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Patient</t>
+    <t>element:Patient.birthDate</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>